<commit_message>
added all tests from design requirments
</commit_message>
<xml_diff>
--- a/DesignRequriments.xlsx
+++ b/DesignRequriments.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24613"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A89FC43-AFB4-4EE9-A89A-0DB19268C4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{266D70A5-2D35-4F0A-869C-F5538037FCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Requirement mark</t>
   </si>
@@ -52,7 +52,7 @@
     <t>1.2.2</t>
   </si>
   <si>
-    <t>If username input is empty display message "Epic sadface: Username is required"</t>
+    <t>If username input is empty and login button is clicked display message "Epic sadface: Username is required"</t>
   </si>
   <si>
     <t>1.2.3</t>
@@ -73,19 +73,13 @@
     <t>2.1.1</t>
   </si>
   <si>
-    <t>Clicking on add to cart should add item to the cart</t>
+    <t>Clicking on add to cart should add item to the cart and display remove button</t>
   </si>
   <si>
     <t>2.1.2</t>
   </si>
   <si>
-    <t>Clicking on add to cart should add iten to the cart and display remove button</t>
-  </si>
-  <si>
-    <t>2.1.3</t>
-  </si>
-  <si>
-    <t>Clicking on add to cart should add iten to the cart and display remove button and clicking remove button should remove item from the cart</t>
+    <t>Clicking on add to cart should add item to the cart and display remove button and clicking remove button should remove item from the cart</t>
   </si>
   <si>
     <t>2.2.1</t>
@@ -545,7 +539,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -626,7 +620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="25.5">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -650,13 +644,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="25.5">
-      <c r="A13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>23</v>
-      </c>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="3"/>

</xml_diff>